<commit_message>
Hoang add 2 chuc nang ql HoiVien: - NhapHOiVien (100%). - CapNhatHoiVien (100%). * Bo sung storeprocedue cho bang CHUC_VU
</commit_message>
<xml_diff>
--- a/4.WBS/WBS.xlsx
+++ b/4.WBS/WBS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>Công việc</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Giao diện có thể tùy chỉnh lại theo ý muốn (có báo lại cho nhóm)</t>
+  </si>
+  <si>
+    <t>Có thay đổi giao diện</t>
   </si>
 </sst>
 </file>
@@ -273,32 +276,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -612,44 +617,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -668,43 +673,43 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="4"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -721,43 +726,47 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="4"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -770,11 +779,15 @@
       <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="4"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
@@ -791,120 +804,120 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="17.25" thickTop="1"/>
     <row r="21" spans="1:7">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B2:E3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Hoang thêm chức năng Tra Cứu HộiViên (90%) - Hỗ trợ nhiều tiêu chí tra cứu khác nhau. - Tiêu chí tra cứu theo HoTen có một chút vấn đề (ví dụ các tên có dấu như: Huyền, Nguyễn,... ko tra cứu được ??) - Một số tiêu chí chưa làm được do chưa có dữ liệu.
</commit_message>
<xml_diff>
--- a/4.WBS/WBS.xlsx
+++ b/4.WBS/WBS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Công việc</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Có thay đổi giao diện</t>
+  </si>
+  <si>
+    <t>Một số chuỗi HoTen ko tra cứu được ??. Một số chức năng sẽ bổ sung sau.</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -290,6 +293,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -299,11 +307,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +605,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -617,18 +621,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
@@ -654,7 +658,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -673,7 +677,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -690,7 +694,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -709,7 +713,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="11"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -726,7 +730,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
@@ -743,7 +747,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -758,7 +762,7 @@
       <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="9">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -766,7 +770,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="11"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -779,7 +783,7 @@
       <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -787,7 +791,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="11"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
@@ -800,11 +804,13 @@
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -817,11 +823,15 @@
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -840,7 +850,7 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
@@ -857,7 +867,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -876,7 +886,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A18" s="10"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
@@ -912,12 +922,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Hoang add 4 nhom chuc nang sau: 1. ql VaiTro (ChucVu) 2. ql LoaiHoiVienBUS 3. ql ChuyenMon (loai ChuyenMon) 4. ql CapBac (loai CapBac) => Co thay doi giao dien MainFrm (tam thoi).
Bo sung CSDL cho cac bang sau:
+ Them bang CHUYEN_MON
+ Them bang CAP_BAC
</commit_message>
<xml_diff>
--- a/4.WBS/WBS.xlsx
+++ b/4.WBS/WBS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
   <si>
     <t>Công việc</t>
   </si>
@@ -139,6 +139,68 @@
   </si>
   <si>
     <t>Một số chuỗi HoTen ko tra cứu được ??. Một số chức năng sẽ bổ sung sau.</t>
+  </si>
+  <si>
+    <t>Quản lý loại hội viên</t>
+  </si>
+  <si>
+    <t>Thêm loại hội viên</t>
+  </si>
+  <si>
+    <t>Xoá loại hội viên</t>
+  </si>
+  <si>
+    <t>Sửa loại hội viên</t>
+  </si>
+  <si>
+    <t>Quản lý chuyên môn</t>
+  </si>
+  <si>
+    <t>Thêm chuyên môn</t>
+  </si>
+  <si>
+    <t>Xoá chuyên môn</t>
+  </si>
+  <si>
+    <t>Sửa chuyên môn</t>
+  </si>
+  <si>
+    <t>Quản lý cấp bậc 
+(thứ hạng)</t>
+  </si>
+  <si>
+    <t>Thêm cấp bậc</t>
+  </si>
+  <si>
+    <t>Xoá cấp bậc</t>
+  </si>
+  <si>
+    <t>Sửa câp bậc</t>
+  </si>
+  <si>
+    <t>Tra cứu cấp bậc theo chuyên môn</t>
+  </si>
+  <si>
+    <t>Quản lý vai trò
+(Chức vụ quản lý)</t>
+  </si>
+  <si>
+    <t>Thêm vai trò</t>
+  </si>
+  <si>
+    <t>Xoá vai trò</t>
+  </si>
+  <si>
+    <t>Sửa vai trò</t>
+  </si>
+  <si>
+    <t>1. Thêm giao diện</t>
+  </si>
+  <si>
+    <t>2. Thay đổi MainFrm</t>
+  </si>
+  <si>
+    <t>3. Lê Long check lại giao diện MainFrm cho phù hợp.</t>
   </si>
 </sst>
 </file>
@@ -187,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -275,11 +337,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -295,19 +370,25 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -621,18 +702,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
@@ -658,7 +739,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -694,7 +775,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -713,7 +794,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="14"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -747,7 +828,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -770,7 +851,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="14"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -791,7 +872,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
@@ -823,7 +904,7 @@
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="11">
         <v>0.9</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -831,103 +912,368 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A19" s="12"/>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A24" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A25" s="12"/>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" thickTop="1" thickBot="1">
+      <c r="A27" s="12"/>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A28" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="5" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A29" s="13"/>
+      <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="D29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="17.25" thickTop="1">
-      <c r="A17" s="14" t="s">
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="17.25" thickTop="1">
+      <c r="A30" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="5" t="s">
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="17.25" thickBot="1">
+      <c r="A31" s="13"/>
+      <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="17.25" thickTop="1"/>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8" t="s">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="17.25" thickTop="1"/>
+    <row r="34" spans="1:2">
+      <c r="A34" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="8" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="7" t="s">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B36" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A17:A18"/>
+  <mergeCells count="10">
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>